<commit_message>
GDP by Industries USA - IoP by Industries UK
</commit_message>
<xml_diff>
--- a/Mergers_Acquisitions/raw/large_acquisitions_in _manufacturing_and_mining_1948_1979_ftc.xlsx
+++ b/Mergers_Acquisitions/raw/large_acquisitions_in _manufacturing_and_mining_1948_1979_ftc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usachcl-my.sharepoint.com/personal/tomas_bustamante_h_usach_cl/Documents/Banco_Central/Mergers_Acquisitions/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4E84ED2-DCEA-464B-A437-9E6C5BE3C02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{C4E84ED2-DCEA-464B-A437-9E6C5BE3C02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{530F6C9A-EA09-4D78-9E14-7E02F8EFD967}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{74801F44-70D1-4101-B575-544BA3B71762}"/>
+    <workbookView xWindow="6480" yWindow="2490" windowWidth="21600" windowHeight="11295" xr2:uid="{74801F44-70D1-4101-B575-544BA3B71762}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <t>n_acq</t>
   </si>
   <si>
-    <t>Assets _M</t>
+    <t>assets _m</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:D34"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>